<commit_message>
ConntectController opgeschoond en overzicht.xls bijgewerkt
</commit_message>
<xml_diff>
--- a/Requirements en User Stories/Overzicht.xlsx
+++ b/Requirements en User Stories/Overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Make IT Work\SofaBank\Requirements en User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651AB8F5-51C4-407B-8F94-ACDC0AC5BCFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6434C95B-CE62-452B-B5BB-F824C4AB7594}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8616" yWindow="3240" windowWidth="17280" windowHeight="8964" xr2:uid="{03E509FD-5BD6-4A12-90A4-D70E3214D998}"/>
+    <workbookView xWindow="-8436" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{03E509FD-5BD6-4A12-90A4-D70E3214D998}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="174">
   <si>
     <t>Index.html</t>
   </si>
@@ -326,9 +326,6 @@
     <t>zie userstories</t>
   </si>
   <si>
-    <t>connect_client.html</t>
-  </si>
-  <si>
     <t>money_transfer.html</t>
   </si>
   <si>
@@ -485,9 +482,6 @@
     <t>ClientView.procesNewBusinessAccount</t>
   </si>
   <si>
-    <t>POST "ConnectToClient"?</t>
-  </si>
-  <si>
     <t>POST "Updateclient" ? Wordt aan gewerkt</t>
   </si>
   <si>
@@ -501,6 +495,63 @@
   </si>
   <si>
     <t>POST "newBusinessAccountHandler"?</t>
+  </si>
+  <si>
+    <t>POST "ConnectAccount"</t>
+  </si>
+  <si>
+    <t>ConnectController</t>
+  </si>
+  <si>
+    <t>connectAccounts(@RequestParam int id, Model model)</t>
+  </si>
+  <si>
+    <t>ConnectingService</t>
+  </si>
+  <si>
+    <t>connect_accounts</t>
+  </si>
+  <si>
+    <t>connect_accounts.html</t>
+  </si>
+  <si>
+    <t>connectHandeler(@RequestParam Map&lt;String, Object&gt; body, Model model)</t>
+  </si>
+  <si>
+    <t>dashboard_clients</t>
+  </si>
+  <si>
+    <t>indien benaderd met een model gevuld met "account" POST "ConnectForm"</t>
+  </si>
+  <si>
+    <t>indien benaderd met een model gevuld met "connection" POST "ConnectValidate"</t>
+  </si>
+  <si>
+    <t>checkMatch(@RequestParam Map&lt;String, Object&gt; body, Model model)</t>
+  </si>
+  <si>
+    <t>indien codes overeenkomen</t>
+  </si>
+  <si>
+    <t>client_view</t>
+  </si>
+  <si>
+    <t>indien codes niet overeenkomen</t>
+  </si>
+  <si>
+    <t>String met foutmelding "wrong" en Connector "connection"</t>
+  </si>
+  <si>
+    <t>POST "NewConnection" (maar alleen zichtbaar als username van ingelogde user  voorkomt in DB table 'connector'</t>
+  </si>
+  <si>
+    <t>matchAccounts(@RequestParam int id, Model model)</t>
+  </si>
+  <si>
+    <t>ConnectingServices</t>
+  </si>
+  <si>
+    <t>Connector "connection"</t>
   </si>
 </sst>
 </file>
@@ -524,7 +575,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -555,6 +606,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -842,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -851,89 +908,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -953,15 +947,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,9 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1004,12 +986,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1027,27 +1003,121 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1363,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED02DC78-24D0-495A-9906-77B9D95F6466}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:G49"/>
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,45 +1447,45 @@
     <col min="4" max="4" width="30.21875" customWidth="1"/>
     <col min="5" max="5" width="20.21875" customWidth="1"/>
     <col min="6" max="6" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="75" t="s">
+      <c r="G2" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="56" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1436,7 +1506,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="56" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1457,7 +1527,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="56" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1478,7 +1548,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="56" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1499,7 +1569,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="56" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1521,41 +1591,41 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="77" t="s">
+      <c r="F10" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="80" t="s">
+      <c r="G10" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1571,12 +1641,12 @@
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1592,12 +1662,12 @@
       <c r="F12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1613,12 +1683,12 @@
       <c r="F13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1634,104 +1704,104 @@
       <c r="F14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="68" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="12" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="79" t="s">
+      <c r="D20" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="77" t="s">
+      <c r="F20" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="80" t="s">
+      <c r="G20" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1747,12 +1817,12 @@
       <c r="F21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1768,12 +1838,12 @@
       <c r="F22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1789,12 +1859,12 @@
       <c r="F23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1810,55 +1880,55 @@
       <c r="F24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="6" t="s">
+      <c r="A26" s="71"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="6" t="s">
+      <c r="A27" s="71"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1867,94 +1937,94 @@
       <c r="F27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="12" t="s">
+      <c r="A28" s="75"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="76" t="s">
+      <c r="A31" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="78" t="s">
+      <c r="C31" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="79" t="s">
+      <c r="D31" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="77" t="s">
+      <c r="E31" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="77" t="s">
+      <c r="F31" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="80" t="s">
+      <c r="G31" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65" t="s">
+      <c r="D32" s="40"/>
+      <c r="E32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="65" t="s">
+      <c r="F32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="67" t="s">
+      <c r="G32" s="42" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="68"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="43"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="64" t="s">
+      <c r="A34" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1970,12 +2040,12 @@
       <c r="F34" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1991,12 +2061,12 @@
       <c r="F35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2012,55 +2082,55 @@
       <c r="F36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="G37" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="27"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="6" t="s">
+      <c r="A38" s="71"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="28" t="s">
+      <c r="G38" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="27"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="6" t="s">
+      <c r="A39" s="71"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -2069,46 +2139,46 @@
       <c r="F39" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="58"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="45"/>
+      <c r="A40" s="72"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="B41" s="61" t="s">
+      <c r="A41" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="63"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="38"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="24"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2126,12 +2196,12 @@
       <c r="F44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2149,18 +2219,18 @@
       <c r="F45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G45" s="28" t="s">
+      <c r="G45" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="65" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="3"/>
@@ -2170,105 +2240,105 @@
       <c r="F46" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="89"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="8"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="85" t="s">
+      <c r="A48" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="86" t="s">
+      <c r="B48" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="86" t="s">
+      <c r="C48" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="56" t="s">
+      <c r="D48" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="F48" s="56" t="s">
+      <c r="F48" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="G48" s="87" t="s">
+      <c r="G48" s="57" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="88"/>
-      <c r="B49" s="89"/>
-      <c r="C49" s="89"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="63"/>
+      <c r="A49" s="83"/>
+      <c r="B49" s="88"/>
+      <c r="C49" s="88"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="38"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="24"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="60"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="77" t="s">
+      <c r="B52" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="77" t="s">
+      <c r="C52" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="79" t="s">
+      <c r="D52" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="77" t="s">
+      <c r="E52" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F52" s="77" t="s">
+      <c r="F52" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G52" s="80" t="s">
+      <c r="G52" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
-        <v>121</v>
+      <c r="A53" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="4"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="8"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D54" s="3" t="s">
@@ -2277,21 +2347,21 @@
       <c r="E54" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F54" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D55" s="3" t="s">
@@ -2300,21 +2370,21 @@
       <c r="E55" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F55" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G55" s="28" t="s">
+      <c r="G55" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D56" s="3" t="s">
@@ -2326,767 +2396,910 @@
       <c r="F56" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G56" s="28" t="s">
+      <c r="G56" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="52" t="s">
+    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="94" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="G57" s="93" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="54" t="s">
+    </row>
+    <row r="59" spans="1:7" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="27"/>
+    </row>
+    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A60" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="60"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A65" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" s="85"/>
+      <c r="C65" s="85"/>
+      <c r="D65" s="85"/>
+      <c r="E65" s="85"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="86"/>
+    </row>
+    <row r="66" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E66" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="D57" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="55" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="50"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="51"/>
-    </row>
-    <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="24"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="76" t="s">
+      <c r="B69" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="33"/>
+      <c r="D69" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+    </row>
+    <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="26"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+    </row>
+    <row r="72" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A72" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" s="85"/>
+      <c r="C72" s="85"/>
+      <c r="D72" s="85"/>
+      <c r="E72" s="85"/>
+      <c r="F72" s="85"/>
+      <c r="G72" s="86"/>
+    </row>
+    <row r="73" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="77" t="s">
+      <c r="B73" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="77" t="s">
+      <c r="C73" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D60" s="79" t="s">
+      <c r="D73" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="77" t="s">
+      <c r="E73" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F60" s="77" t="s">
+      <c r="F73" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G60" s="80" t="s">
+      <c r="G73" s="50" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+    <row r="74" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" s="90"/>
+      <c r="C74" s="90"/>
+      <c r="D74" s="91"/>
+      <c r="E74" s="90"/>
+      <c r="F74" s="90"/>
+      <c r="G74" s="90"/>
+    </row>
+    <row r="75" spans="1:7" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="92" t="s">
+        <v>163</v>
+      </c>
+      <c r="B75" s="90" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="92" t="s">
+        <v>161</v>
+      </c>
+      <c r="D75" s="91" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75" s="90" t="s">
+        <v>158</v>
+      </c>
+      <c r="F75" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="G75" s="90" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="92" t="s">
+        <v>164</v>
+      </c>
+      <c r="B76" s="90" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="92" t="s">
+        <v>165</v>
+      </c>
+      <c r="D76" s="91" t="s">
+        <v>166</v>
+      </c>
+      <c r="E76" s="90" t="s">
+        <v>158</v>
+      </c>
+      <c r="F76" s="92" t="s">
+        <v>85</v>
+      </c>
+      <c r="G76" s="90" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="92"/>
+      <c r="B77" s="90"/>
+      <c r="C77" s="92"/>
+      <c r="D77" s="91" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="92" t="s">
+        <v>169</v>
+      </c>
+      <c r="G77" s="90" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+    </row>
+    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A79" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B79" s="59"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="59"/>
+      <c r="F79" s="59"/>
+      <c r="G79" s="60"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F80" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="7"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="71"/>
+      <c r="B83" s="78"/>
+      <c r="C83" s="80"/>
+      <c r="D83" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="71"/>
+      <c r="B84" s="78"/>
+      <c r="C84" s="80"/>
+      <c r="D84" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="71"/>
+      <c r="B85" s="78"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="71"/>
+      <c r="B86" s="78"/>
+      <c r="C86" s="80"/>
+      <c r="D86" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="75"/>
+      <c r="B87" s="79"/>
+      <c r="C87" s="81"/>
+      <c r="D87" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G87" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A89" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" s="62"/>
+      <c r="C89" s="62"/>
+      <c r="D89" s="62"/>
+      <c r="E89" s="62"/>
+      <c r="F89" s="62"/>
+      <c r="G89" s="62"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E90" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F90" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90" s="50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F92" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A94" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B94" s="62"/>
+      <c r="C94" s="62"/>
+      <c r="D94" s="62"/>
+      <c r="E94" s="62"/>
+      <c r="F94" s="62"/>
+      <c r="G94" s="62"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D95" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E95" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F95" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G95" s="50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="8"/>
-    </row>
-    <row r="62" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="48"/>
-    </row>
-    <row r="65" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="77" t="s">
+      <c r="B97" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="99" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A99" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B99" s="59"/>
+      <c r="C99" s="59"/>
+      <c r="D99" s="59"/>
+      <c r="E99" s="59"/>
+      <c r="F99" s="59"/>
+      <c r="G99" s="60"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="77" t="s">
+      <c r="B100" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="77" t="s">
+      <c r="C100" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D65" s="79" t="s">
+      <c r="D100" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E65" s="77" t="s">
+      <c r="E100" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F65" s="77" t="s">
+      <c r="F100" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G65" s="77" t="s">
+      <c r="G100" s="53" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-    </row>
-    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D67" s="3" t="s">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="7"/>
+    </row>
+    <row r="102" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A102" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="B68" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68" s="57"/>
-      <c r="D68" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="E68" s="56"/>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="B69" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="34"/>
-    </row>
-    <row r="71" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A71" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="24"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="76" t="s">
+      <c r="E103" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G103" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A105" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B105" s="59"/>
+      <c r="C105" s="59"/>
+      <c r="D105" s="59"/>
+      <c r="E105" s="59"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="60"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="77" t="s">
+      <c r="B106" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="77" t="s">
+      <c r="C106" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D72" s="79" t="s">
+      <c r="D106" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E72" s="77" t="s">
+      <c r="E106" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F72" s="77" t="s">
+      <c r="F106" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G72" s="80" t="s">
+      <c r="G106" s="53" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="8"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E74" s="3" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B107" s="22"/>
+      <c r="C107" s="22"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="24"/>
+    </row>
+    <row r="108" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G74" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="27"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="27"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="27"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G77" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="27"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" s="3" t="s">
+      <c r="E108" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="29"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E79" s="12" t="s">
+      <c r="E109" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="111" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A111" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111" s="59"/>
+      <c r="C111" s="59"/>
+      <c r="D111" s="59"/>
+      <c r="E111" s="59"/>
+      <c r="F111" s="59"/>
+      <c r="G111" s="60"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B112" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C112" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D112" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E112" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F112" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="G79" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A81" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B82" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C82" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="D82" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="E82" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F82" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G82" s="77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B84" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D84" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F84" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="G84" s="40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A86" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B87" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C87" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="D87" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="E87" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F87" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G87" s="77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B89" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="91" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A91" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B91" s="23"/>
-      <c r="C91" s="23"/>
-      <c r="D91" s="23"/>
-      <c r="E91" s="23"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="24"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B92" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C92" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="D92" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="E92" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F92" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G92" s="80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="8"/>
-    </row>
-    <row r="94" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A94" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G94" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G95" s="33" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="97" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A97" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B97" s="23"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="24"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C98" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="D98" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="E98" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F98" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G98" s="80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="B99" s="43"/>
-      <c r="C99" s="43"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="43"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="45"/>
-    </row>
-    <row r="100" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A100" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F100" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="103" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A103" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B103" s="23"/>
-      <c r="C103" s="23"/>
-      <c r="D103" s="23"/>
-      <c r="E103" s="23"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="24"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B104" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C104" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="D104" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="E104" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F104" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G104" s="80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="81"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="13"/>
-    </row>
-    <row r="108" spans="1:7" s="50" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A108" s="82"/>
-      <c r="B108" s="82"/>
-      <c r="C108" s="82"/>
-      <c r="D108" s="82"/>
-      <c r="E108" s="82"/>
-      <c r="F108" s="82"/>
-      <c r="G108" s="82"/>
-    </row>
-    <row r="109" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D109" s="83"/>
-    </row>
-    <row r="110" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D110" s="83"/>
-    </row>
-    <row r="111" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C111" s="51"/>
-      <c r="D111" s="51"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="54"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="10"/>
+    </row>
+    <row r="116" spans="1:7" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A116" s="61"/>
+      <c r="B116" s="61"/>
+      <c r="C116" s="61"/>
+      <c r="D116" s="61"/>
+      <c r="E116" s="61"/>
+      <c r="F116" s="61"/>
+      <c r="G116" s="61"/>
+    </row>
+    <row r="117" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D117" s="55"/>
+    </row>
+    <row r="118" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D118" s="55"/>
+    </row>
+    <row r="119" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A108:G108"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A86:G86"/>
-    <mergeCell ref="A91:G91"/>
-    <mergeCell ref="A97:G97"/>
-    <mergeCell ref="A103:G103"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A9:G9"/>
+  <mergeCells count="35">
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="C37:C40"/>
@@ -3096,19 +3309,23 @@
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B74:B79"/>
-    <mergeCell ref="C74:C79"/>
-    <mergeCell ref="A74:A79"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A116:G116"/>
+    <mergeCell ref="A89:G89"/>
+    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="A99:G99"/>
+    <mergeCell ref="A105:G105"/>
+    <mergeCell ref="A111:G111"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="C82:C87"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="A79:G79"/>
+    <mergeCell ref="A72:G72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
code wat opgeschoond en overzicht.xls bijgewerkt
</commit_message>
<xml_diff>
--- a/Requirements en User Stories/Overzicht.xlsx
+++ b/Requirements en User Stories/Overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Make IT Work\SofaBank\Requirements en User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6434C95B-CE62-452B-B5BB-F824C4AB7594}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BCEDBE-21F7-442A-8CA7-38CFDCDC3FF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8436" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{03E509FD-5BD6-4A12-90A4-D70E3214D998}"/>
+    <workbookView xWindow="0" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{03E509FD-5BD6-4A12-90A4-D70E3214D998}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="184">
   <si>
     <t>Index.html</t>
   </si>
@@ -467,30 +467,6 @@
     <t>dashboard_employee.html</t>
   </si>
   <si>
-    <t>POST "NewBusiness"</t>
-  </si>
-  <si>
-    <t>ClientviewController</t>
-  </si>
-  <si>
-    <t>newBAccount(Business business, Model model)</t>
-  </si>
-  <si>
-    <t>Nog geen, maar kunnen nog worden uitgebreid</t>
-  </si>
-  <si>
-    <t>ClientView.procesNewBusinessAccount</t>
-  </si>
-  <si>
-    <t>POST "Updateclient" ? Wordt aan gewerkt</t>
-  </si>
-  <si>
-    <t>nog niet bekend</t>
-  </si>
-  <si>
-    <t>update_client.html?</t>
-  </si>
-  <si>
     <t>POST "AddPDQ"?</t>
   </si>
   <si>
@@ -552,6 +528,60 @@
   </si>
   <si>
     <t>Connector "connection"</t>
+  </si>
+  <si>
+    <t>POST "updateHandler"</t>
+  </si>
+  <si>
+    <t>POST "changeAddressForm"</t>
+  </si>
+  <si>
+    <t>PersonalPageController</t>
+  </si>
+  <si>
+    <t>updateHandler(@RequestParam int id, Model model)</t>
+  </si>
+  <si>
+    <t>UpdateClient</t>
+  </si>
+  <si>
+    <t>edit_client_personalpage.html</t>
+  </si>
+  <si>
+    <t>changeAddress(@RequestParam int clientId, @RequestParam int addressId, Model model)</t>
+  </si>
+  <si>
+    <t>Address "address", ClientId "clientId"</t>
+  </si>
+  <si>
+    <t>change_address.html</t>
+  </si>
+  <si>
+    <t>edit_client_personalPage.html</t>
+  </si>
+  <si>
+    <t>POST "updateClient"</t>
+  </si>
+  <si>
+    <t>processUpdate(@RequestParam Map&lt;String, Object&gt; input, Model model)</t>
+  </si>
+  <si>
+    <t>indien username ongewijzigd is, cq gekozen username al ingebruik was en dus niet kon worden gewijzigd.</t>
+  </si>
+  <si>
+    <t>updateClient</t>
+  </si>
+  <si>
+    <t>foutmelding "username", Client "client", Account "account"</t>
+  </si>
+  <si>
+    <t>indien username is gewijzigd</t>
+  </si>
+  <si>
+    <t>POST "changeAddress"</t>
+  </si>
+  <si>
+    <t>processAddress(@RequestParam Map&lt;String, String&gt; input, @RequestParam int clientId, Model model)</t>
   </si>
 </sst>
 </file>
@@ -613,7 +643,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -895,11 +925,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -952,14 +1026,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1010,102 +1078,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1119,6 +1091,118 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1433,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED02DC78-24D0-495A-9906-77B9D95F6466}">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,45 +1531,45 @@
     <col min="4" max="4" width="30.21875" customWidth="1"/>
     <col min="5" max="5" width="20.21875" customWidth="1"/>
     <col min="6" max="6" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="46" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1506,7 +1590,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1527,7 +1611,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="54" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1548,7 +1632,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="54" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1569,7 +1653,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1591,41 +1675,41 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="63"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="51" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1646,7 +1730,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1667,7 +1751,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1688,7 +1772,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1709,13 +1793,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1732,9 +1816,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="69"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
@@ -1749,9 +1833,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="64"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="70"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="9" t="s">
         <v>37</v>
       </c>
@@ -1767,41 +1851,41 @@
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="60"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="53" t="s">
+      <c r="G20" s="51" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1822,7 +1906,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1843,7 +1927,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1864,7 +1948,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1885,13 +1969,13 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="68" t="s">
+      <c r="C25" s="81" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1908,9 +1992,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="71"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="69"/>
+      <c r="A26" s="74"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="82"/>
       <c r="D26" s="5" t="s">
         <v>49</v>
       </c>
@@ -1925,9 +2009,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="71"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="69"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="82"/>
       <c r="D27" s="5" t="s">
         <v>37</v>
       </c>
@@ -1942,9 +2026,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="75"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="70"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="83"/>
       <c r="D28" s="9" t="s">
         <v>59</v>
       </c>
@@ -1960,71 +2044,71 @@
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="60"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="63"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="50" t="s">
+      <c r="F31" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="53" t="s">
+      <c r="G31" s="51" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40" t="s">
+      <c r="D32" s="38"/>
+      <c r="E32" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="42" t="s">
+      <c r="G32" s="40" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="77"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="43"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="41"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2045,7 +2129,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2066,7 +2150,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2087,13 +2171,13 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="71" t="s">
+      <c r="A37" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="73" t="s">
+      <c r="C37" s="77" t="s">
         <v>61</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -2110,9 +2194,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="71"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="74"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="5" t="s">
         <v>64</v>
       </c>
@@ -2127,9 +2211,9 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="71"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="74"/>
+      <c r="A39" s="74"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="5" t="s">
         <v>66</v>
       </c>
@@ -2144,38 +2228,38 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="72"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="34"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
       <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="36" t="s">
+      <c r="A41" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="37"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="38"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="58" t="s">
+      <c r="A43" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="60"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="63"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
@@ -2224,13 +2308,13 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="65" t="s">
+      <c r="B46" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="65" t="s">
+      <c r="C46" s="72" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="3"/>
@@ -2245,78 +2329,78 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="63"/>
-      <c r="B47" s="89"/>
-      <c r="C47" s="89"/>
+      <c r="A47" s="64"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="73"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="82" t="s">
+      <c r="A48" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="87" t="s">
+      <c r="B48" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="87" t="s">
+      <c r="C48" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="32" t="s">
+      <c r="D48" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="32" t="s">
+      <c r="E48" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="F48" s="32" t="s">
+      <c r="F48" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G48" s="57" t="s">
+      <c r="G48" s="55" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="83"/>
-      <c r="B49" s="88"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="38"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="59"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="60"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="63"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="50" t="s">
+      <c r="C52" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="52" t="s">
+      <c r="D52" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="50" t="s">
+      <c r="E52" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F52" s="50" t="s">
+      <c r="F52" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G52" s="53" t="s">
+      <c r="G52" s="51" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2401,905 +2485,1161 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="94" t="s">
-        <v>170</v>
+      <c r="A57" s="60" t="s">
+        <v>162</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C57" s="34" t="s">
-        <v>171</v>
+        <v>148</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>163</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>70</v>
       </c>
       <c r="E57" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="G57" s="59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="D58" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G57" s="93" t="s">
+      <c r="G58" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="93"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="94"/>
+      <c r="F60" s="94"/>
+      <c r="G60" s="96"/>
+    </row>
+    <row r="61" spans="1:7" s="25" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A61" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="63"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E62" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="97"/>
+      <c r="B66" s="98"/>
+      <c r="C66" s="99"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="98"/>
+      <c r="F66" s="99"/>
+      <c r="G66" s="100"/>
+    </row>
+    <row r="67" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A67" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="B67" s="62"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="63"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E68" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" s="51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="7"/>
+    </row>
+    <row r="70" spans="1:7" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="26"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="27"/>
+    </row>
+    <row r="73" spans="1:7" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A73" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" s="62"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="63"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F74" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="1:7" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A78" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78" s="68"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="68"/>
+      <c r="F78" s="68"/>
+      <c r="G78" s="69"/>
+    </row>
+    <row r="79" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F79" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79" s="48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="1:7" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" s="31"/>
+      <c r="D82" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E82" s="30"/>
+      <c r="F82" s="30"/>
+      <c r="G82" s="30"/>
+    </row>
+    <row r="83" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="26"/>
+    </row>
+    <row r="85" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A85" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="B85" s="68"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68"/>
+      <c r="F85" s="68"/>
+      <c r="G85" s="69"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D86" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E86" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F86" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" s="56"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="57"/>
+      <c r="E87" s="56"/>
+      <c r="F87" s="56"/>
+      <c r="G87" s="56"/>
+    </row>
+    <row r="88" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="B88" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C88" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="D88" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F88" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="G88" s="56" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="B89" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C89" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="D89" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="E89" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F89" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="G89" s="56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="58"/>
+      <c r="B90" s="56"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="57" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="30" t="s">
+      <c r="E90" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="G90" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="D58" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="27"/>
-    </row>
-    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A60" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="60"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="49" t="s">
+    </row>
+    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="15"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+    </row>
+    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A92" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B92" s="62"/>
+      <c r="C92" s="62"/>
+      <c r="D92" s="62"/>
+      <c r="E92" s="62"/>
+      <c r="F92" s="62"/>
+      <c r="G92" s="63"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B93" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="50" t="s">
+      <c r="C93" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D61" s="52" t="s">
+      <c r="D93" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E61" s="50" t="s">
+      <c r="E93" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F61" s="50" t="s">
+      <c r="F93" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G61" s="53" t="s">
+      <c r="G93" s="51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A65" s="84" t="s">
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="7"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="89" t="s">
+        <v>100</v>
+      </c>
+      <c r="C95" s="91" t="s">
+        <v>101</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="74"/>
+      <c r="B96" s="89"/>
+      <c r="C96" s="91"/>
+      <c r="D96" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A97" s="74"/>
+      <c r="B97" s="89"/>
+      <c r="C97" s="91"/>
+      <c r="D97" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A98" s="74"/>
+      <c r="B98" s="89"/>
+      <c r="C98" s="91"/>
+      <c r="D98" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A99" s="74"/>
+      <c r="B99" s="89"/>
+      <c r="C99" s="91"/>
+      <c r="D99" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="79"/>
+      <c r="B100" s="90"/>
+      <c r="C100" s="92"/>
+      <c r="D100" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G100" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A102" s="88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" s="88"/>
+      <c r="C102" s="88"/>
+      <c r="D102" s="88"/>
+      <c r="E102" s="88"/>
+      <c r="F102" s="88"/>
+      <c r="G102" s="88"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B103" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E103" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F103" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103" s="48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G105" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B65" s="85"/>
-      <c r="C65" s="85"/>
-      <c r="D65" s="85"/>
-      <c r="E65" s="85"/>
-      <c r="F65" s="85"/>
-      <c r="G65" s="86"/>
-    </row>
-    <row r="66" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="50" t="s">
+    </row>
+    <row r="107" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A107" s="88" t="s">
+        <v>51</v>
+      </c>
+      <c r="B107" s="88"/>
+      <c r="C107" s="88"/>
+      <c r="D107" s="88"/>
+      <c r="E107" s="88"/>
+      <c r="F107" s="88"/>
+      <c r="G107" s="88"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="50" t="s">
+      <c r="B108" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="50" t="s">
+      <c r="C108" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="D108" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E66" s="50" t="s">
+      <c r="E108" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F66" s="50" t="s">
+      <c r="F108" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="50" t="s">
+      <c r="G108" s="48" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D68" s="3" t="s">
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A112" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="B112" s="62"/>
+      <c r="C112" s="62"/>
+      <c r="D112" s="62"/>
+      <c r="E112" s="62"/>
+      <c r="F112" s="62"/>
+      <c r="G112" s="63"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B113" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D113" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E113" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F113" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113" s="51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="7"/>
+    </row>
+    <row r="115" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A115" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="B69" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="33"/>
-      <c r="D69" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="32"/>
-    </row>
-    <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D70" s="3" t="s">
+      <c r="E116" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G116" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="118" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A118" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118" s="62"/>
+      <c r="C118" s="62"/>
+      <c r="D118" s="62"/>
+      <c r="E118" s="62"/>
+      <c r="F118" s="62"/>
+      <c r="G118" s="63"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D119" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E119" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F119" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G119" s="51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="22"/>
+      <c r="C120" s="22"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="22"/>
+      <c r="F120" s="22"/>
+      <c r="G120" s="24"/>
+    </row>
+    <row r="121" spans="1:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A121" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
-    </row>
-    <row r="72" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A72" s="84" t="s">
-        <v>160</v>
-      </c>
-      <c r="B72" s="85"/>
-      <c r="C72" s="85"/>
-      <c r="D72" s="85"/>
-      <c r="E72" s="85"/>
-      <c r="F72" s="85"/>
-      <c r="G72" s="86"/>
-    </row>
-    <row r="73" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="50" t="s">
+      <c r="E121" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123"/>
+      <c r="B123"/>
+      <c r="C123"/>
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123"/>
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A124" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B124" s="62"/>
+      <c r="C124" s="62"/>
+      <c r="D124" s="62"/>
+      <c r="E124" s="62"/>
+      <c r="F124" s="62"/>
+      <c r="G124" s="63"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="50" t="s">
+      <c r="B125" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="50" t="s">
+      <c r="C125" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="52" t="s">
+      <c r="D125" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E73" s="50" t="s">
+      <c r="E125" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F73" s="50" t="s">
+      <c r="F125" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G73" s="50" t="s">
+      <c r="G125" s="51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="90" t="s">
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="90"/>
-      <c r="C74" s="90"/>
-      <c r="D74" s="91"/>
-      <c r="E74" s="90"/>
-      <c r="F74" s="90"/>
-      <c r="G74" s="90"/>
-    </row>
-    <row r="75" spans="1:7" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="92" t="s">
-        <v>163</v>
-      </c>
-      <c r="B75" s="90" t="s">
-        <v>156</v>
-      </c>
-      <c r="C75" s="92" t="s">
-        <v>161</v>
-      </c>
-      <c r="D75" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="E75" s="90" t="s">
-        <v>158</v>
-      </c>
-      <c r="F75" s="90" t="s">
-        <v>89</v>
-      </c>
-      <c r="G75" s="90" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="92" t="s">
-        <v>164</v>
-      </c>
-      <c r="B76" s="90" t="s">
-        <v>156</v>
-      </c>
-      <c r="C76" s="92" t="s">
-        <v>165</v>
-      </c>
-      <c r="D76" s="91" t="s">
-        <v>166</v>
-      </c>
-      <c r="E76" s="90" t="s">
-        <v>158</v>
-      </c>
-      <c r="F76" s="92" t="s">
-        <v>85</v>
-      </c>
-      <c r="G76" s="90" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="92"/>
-      <c r="B77" s="90"/>
-      <c r="C77" s="92"/>
-      <c r="D77" s="91" t="s">
-        <v>168</v>
-      </c>
-      <c r="E77" s="90" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="92" t="s">
-        <v>169</v>
-      </c>
-      <c r="G77" s="90" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="15"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-    </row>
-    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A79" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B79" s="59"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="59"/>
-      <c r="E79" s="59"/>
-      <c r="F79" s="59"/>
-      <c r="G79" s="60"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D80" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E80" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F80" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80" s="53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="7"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="B82" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="C82" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="71"/>
-      <c r="B83" s="78"/>
-      <c r="C83" s="80"/>
-      <c r="D83" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="71"/>
-      <c r="B84" s="78"/>
-      <c r="C84" s="80"/>
-      <c r="D84" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="71"/>
-      <c r="B85" s="78"/>
-      <c r="C85" s="80"/>
-      <c r="D85" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="71"/>
-      <c r="B86" s="78"/>
-      <c r="C86" s="80"/>
-      <c r="D86" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="75"/>
-      <c r="B87" s="79"/>
-      <c r="C87" s="81"/>
-      <c r="D87" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G87" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A89" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="B89" s="62"/>
-      <c r="C89" s="62"/>
-      <c r="D89" s="62"/>
-      <c r="E89" s="62"/>
-      <c r="F89" s="62"/>
-      <c r="G89" s="62"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C90" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D90" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E90" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F90" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G90" s="50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-    </row>
-    <row r="92" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F92" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G92" s="19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A94" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="B94" s="62"/>
-      <c r="C94" s="62"/>
-      <c r="D94" s="62"/>
-      <c r="E94" s="62"/>
-      <c r="F94" s="62"/>
-      <c r="G94" s="62"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B95" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D95" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E95" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F95" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G95" s="50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-    </row>
-    <row r="97" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="99" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A99" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B99" s="59"/>
-      <c r="C99" s="59"/>
-      <c r="D99" s="59"/>
-      <c r="E99" s="59"/>
-      <c r="F99" s="59"/>
-      <c r="G99" s="60"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B100" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C100" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D100" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E100" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F100" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G100" s="53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="7"/>
-    </row>
-    <row r="102" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A102" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G102" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G103" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A105" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="B105" s="59"/>
-      <c r="C105" s="59"/>
-      <c r="D105" s="59"/>
-      <c r="E105" s="59"/>
-      <c r="F105" s="59"/>
-      <c r="G105" s="60"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B106" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C106" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D106" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E106" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F106" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G106" s="53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="22"/>
-      <c r="D107" s="23"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="22"/>
-      <c r="G107" s="24"/>
-    </row>
-    <row r="108" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="111" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A111" s="58" t="s">
-        <v>144</v>
-      </c>
-      <c r="B111" s="59"/>
-      <c r="C111" s="59"/>
-      <c r="D111" s="59"/>
-      <c r="E111" s="59"/>
-      <c r="F111" s="59"/>
-      <c r="G111" s="60"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B112" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C112" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D112" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E112" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F112" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G112" s="53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="54"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="10"/>
-    </row>
-    <row r="116" spans="1:7" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A116" s="61"/>
-      <c r="B116" s="61"/>
-      <c r="C116" s="61"/>
-      <c r="D116" s="61"/>
-      <c r="E116" s="61"/>
-      <c r="F116" s="61"/>
-      <c r="G116" s="61"/>
-    </row>
-    <row r="117" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D117" s="55"/>
-    </row>
-    <row r="118" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D118" s="55"/>
-    </row>
-    <row r="119" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C119" s="27"/>
-      <c r="D119" s="27"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="52"/>
+      <c r="E126" s="8"/>
+      <c r="F126" s="8"/>
+      <c r="G126" s="10"/>
+    </row>
+    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A129" s="87"/>
+      <c r="B129" s="87"/>
+      <c r="C129" s="87"/>
+      <c r="D129" s="87"/>
+      <c r="E129" s="87"/>
+      <c r="F129" s="87"/>
+      <c r="G129" s="87"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" s="26"/>
+      <c r="B130" s="26"/>
+      <c r="C130" s="26"/>
+      <c r="D130" s="53"/>
+      <c r="E130" s="26"/>
+      <c r="F130" s="26"/>
+      <c r="G130" s="26"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="26"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="26"/>
+      <c r="D131" s="53"/>
+      <c r="E131" s="26"/>
+      <c r="F131" s="26"/>
+      <c r="G131" s="26"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="26"/>
+      <c r="B132" s="26"/>
+      <c r="C132" s="27"/>
+      <c r="D132" s="27"/>
+      <c r="E132" s="26"/>
+      <c r="F132" s="26"/>
+      <c r="G132" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
+  <mergeCells count="37">
+    <mergeCell ref="B95:B100"/>
+    <mergeCell ref="C95:C100"/>
+    <mergeCell ref="A95:A100"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A85:G85"/>
+    <mergeCell ref="A129:G129"/>
+    <mergeCell ref="A102:G102"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="A112:G112"/>
+    <mergeCell ref="A118:G118"/>
+    <mergeCell ref="A124:G124"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A9:G9"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="C37:C40"/>
@@ -3309,23 +3649,18 @@
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A116:G116"/>
-    <mergeCell ref="A89:G89"/>
-    <mergeCell ref="A94:G94"/>
-    <mergeCell ref="A99:G99"/>
-    <mergeCell ref="A105:G105"/>
-    <mergeCell ref="A111:G111"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="C82:C87"/>
-    <mergeCell ref="A82:A87"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A67:G67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>